<commit_message>
Further progress on camera setting controller
Also made more widgets list dialog.
</commit_message>
<xml_diff>
--- a/design/Widgets list.xlsx
+++ b/design/Widgets list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroscopyInnovation\Documents\GitHub\ASLM\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11C01EA-C949-41CC-A73F-65A37C97720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2FAE3-A467-48EC-8D08-254B4F69EEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="10540" windowWidth="38400" windowHeight="10220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="2030" windowWidth="38400" windowHeight="18190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="260">
   <si>
     <t>view</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>recalculate stack acquistion time and experiment time, update their values</t>
-  </si>
-  <si>
-    <t>disabled</t>
   </si>
   <si>
     <t>stack_cycling_mode</t>
@@ -726,18 +723,9 @@
     <t>If == 'Normal', Readout Direction and Number of Pixels Disabled.</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>model.camera.set_camera_sensor_mode('Normal')</t>
-  </si>
-  <si>
     <t>Top-to-Bottom' or 'Bottom-to-Top'</t>
   </si>
   <si>
-    <t>model.camera.set_camera_readout_direction(string value)</t>
-  </si>
-  <si>
     <t>configuration.CameraParameters['y_pixels']</t>
   </si>
   <si>
@@ -753,24 +741,15 @@
     <t>readout_time</t>
   </si>
   <si>
-    <t>framerate</t>
-  </si>
-  <si>
     <t>images_to_average</t>
   </si>
   <si>
     <t>Retrieve current exposure time for the active channel in milliseconds</t>
   </si>
   <si>
-    <t>model.camera.calculate_camera_readout_time()</t>
-  </si>
-  <si>
     <t>Calculate theoretical time needed to acquire image (exp + readout)</t>
   </si>
   <si>
-    <t>Need a function that actual framerate with computational overhead</t>
-  </si>
-  <si>
     <t>Calculate imaging actual framerate</t>
   </si>
   <si>
@@ -835,13 +814,37 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>configuration.CameraParameters['exposure_time']</t>
+  </si>
+  <si>
+    <t>configuration.CameraParameters['frames_to_average']</t>
+  </si>
+  <si>
+    <t>1 ms</t>
+  </si>
+  <si>
+    <t>model.camera.set_sensor_mode('Normal')</t>
+  </si>
+  <si>
+    <t>model.camera.set_readout_direction(string value)</t>
+  </si>
+  <si>
+    <t>model.camera.calculate_readout_time()</t>
+  </si>
+  <si>
+    <t>max_framerate</t>
+  </si>
+  <si>
+    <t>model.camera_calculate_readout_time()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -927,6 +930,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -981,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1031,6 +1040,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1062,6 +1074,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1285,11 +1306,11 @@
   <dimension ref="A1:AG88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3750" ySplit="3350" topLeftCell="N16" activePane="topRight"/>
-      <selection activeCell="B3" sqref="B3:B5"/>
-      <selection pane="topRight" activeCell="Q9" sqref="Q9"/>
+      <pane xSplit="3750" ySplit="14320" topLeftCell="G1" activePane="topRight"/>
+      <selection activeCell="A3" sqref="A3:A20"/>
+      <selection pane="topRight" activeCell="G47" sqref="G47"/>
       <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
-      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1314,116 +1335,116 @@
     <col min="18" max="16384" width="12.6328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="22" t="s">
+    <row r="1" spans="1:33" s="26" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="22" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="M1" s="22" t="s">
+      <c r="L1" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="M1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-    </row>
-    <row r="2" spans="1:33" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24" t="s">
+      <c r="N1" s="24"/>
+      <c r="O1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+    </row>
+    <row r="2" spans="1:33" s="26" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>238</v>
-      </c>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
     </row>
     <row r="3" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1434,68 +1455,74 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="L3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="N3" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="L3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="O3" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>180</v>
+      <c r="O3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="L4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" s="27" t="s">
         <v>256</v>
       </c>
-      <c r="H4" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="L4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="P4" s="26" t="s">
-        <v>180</v>
+      <c r="O4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1505,120 +1532,141 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>257</v>
+      <c r="E5" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>250</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>180</v>
+        <v>223</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>179</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="L5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="O5" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="P5" s="26" t="s">
-        <v>222</v>
+      <c r="O5" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="28" t="s">
+        <v>252</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="28" t="s">
+        <v>254</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
+      </c>
+      <c r="L6" s="27" t="b">
+        <v>1</v>
       </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="P6" s="27" t="s">
-        <v>180</v>
+      <c r="O6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="28" t="s">
+        <v>251</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="28" t="s">
+        <v>251</v>
+      </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O7" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="28" t="s">
         <v>258</v>
-      </c>
-      <c r="P7" s="27" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="28" t="s">
+        <v>251</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="28" t="s">
+        <v>251</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="O8" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="P8" s="27" t="s">
-        <v>258</v>
+        <v>230</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="O8" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="P8" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
@@ -1626,8 +1674,8 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
+      <c r="E9" s="28" t="s">
+        <v>253</v>
       </c>
       <c r="F9" s="1">
         <v>8</v>
@@ -1639,20 +1687,22 @@
         <v>24</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="2"/>
+      <c r="L9" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="O9" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="P9" s="26" t="s">
-        <v>180</v>
+        <v>238</v>
+      </c>
+      <c r="O9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:33" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1666,7 +1716,7 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1677,78 +1727,92 @@
         <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G11" s="1">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="L11" s="2"/>
+        <v>237</v>
+      </c>
+      <c r="L11" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="M11" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="O11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D12" s="1">
         <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G12" s="1">
         <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="2"/>
+      <c r="N12" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="O12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1756,33 +1820,39 @@
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="O13" s="27" t="s">
         <v>251</v>
       </c>
+      <c r="P13" s="27" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="14" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1790,33 +1860,39 @@
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="O14" s="27" t="s">
         <v>251</v>
       </c>
+      <c r="P14" s="27" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="15" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1833,23 +1909,29 @@
         <v>1024</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>248</v>
+      <c r="O15" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="P15" s="27" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1866,23 +1948,29 @@
         <v>1024</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="N16" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>248</v>
+      <c r="O16" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="P16" s="27" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1890,36 +1978,42 @@
         <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>251</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="O17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="1">
         <v>1600</v>
       </c>
@@ -1927,36 +2021,42 @@
         <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>251</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="O18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="1">
         <v>1024</v>
       </c>
@@ -1964,36 +2064,42 @@
         <v>32</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>251</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="O19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="8">
         <v>512</v>
       </c>
@@ -2001,36 +2107,40 @@
         <v>32</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="J20" s="8"/>
-      <c r="K20" s="8" t="s">
-        <v>241</v>
+      <c r="K20" s="29" t="s">
+        <v>251</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8" t="s">
         <v>33</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
+        <v>241</v>
+      </c>
+      <c r="O20" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P20" s="8" t="b">
+        <v>0</v>
+      </c>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
@@ -2050,7 +2160,7 @@
       <c r="AG20" s="8"/>
     </row>
     <row r="21" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2077,9 +2187,15 @@
       <c r="N21" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="O21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
@@ -2104,9 +2220,15 @@
       <c r="N22" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="O22" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P22" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
@@ -2131,9 +2253,15 @@
       <c r="N23" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="O23" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
@@ -2158,9 +2286,15 @@
       <c r="N24" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="O24" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
@@ -2185,9 +2319,15 @@
       <c r="N25" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="O25" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
@@ -2212,9 +2352,15 @@
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="1"/>
+      <c r="O26" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="1" t="s">
         <v>62</v>
       </c>
@@ -2239,9 +2385,15 @@
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="1"/>
+      <c r="O27" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="1" t="s">
         <v>67</v>
       </c>
@@ -2266,9 +2418,15 @@
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="1"/>
+      <c r="O28" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
@@ -2293,9 +2451,15 @@
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="1"/>
+      <c r="O29" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="1" t="s">
         <v>77</v>
       </c>
@@ -2307,9 +2471,15 @@
       <c r="M30" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="O30" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="1" t="s">
         <v>79</v>
       </c>
@@ -2321,9 +2491,15 @@
       <c r="M31" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="O31" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
@@ -2335,9 +2511,15 @@
       <c r="M32" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="O32" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
@@ -2349,9 +2531,15 @@
       <c r="M33" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="O33" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="1" t="s">
         <v>85</v>
       </c>
@@ -2363,9 +2551,15 @@
       <c r="M34" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="O34" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
@@ -2377,9 +2571,15 @@
       <c r="M35" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="O35" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P35" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="1" t="s">
         <v>88</v>
       </c>
@@ -2391,9 +2591,15 @@
       <c r="M36" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="O36" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P36" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="1" t="s">
         <v>89</v>
       </c>
@@ -2405,9 +2611,15 @@
       <c r="M37" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="O37" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P37" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="1" t="s">
         <v>90</v>
       </c>
@@ -2419,9 +2631,15 @@
       <c r="M38" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="O38" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="1" t="s">
         <v>91</v>
       </c>
@@ -2433,9 +2651,15 @@
       <c r="M39" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="O39" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P39" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="1" t="s">
         <v>92</v>
       </c>
@@ -2445,9 +2669,15 @@
       <c r="M40" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="O40" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P40" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="1" t="s">
         <v>94</v>
       </c>
@@ -2457,9 +2687,15 @@
       <c r="M41" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="O41" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="1" t="s">
         <v>96</v>
       </c>
@@ -2469,9 +2705,15 @@
       <c r="M42" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="O42" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="8" t="s">
         <v>98</v>
       </c>
@@ -2491,8 +2733,12 @@
         <v>99</v>
       </c>
       <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
+      <c r="O43" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P43" s="17" t="b">
+        <v>1</v>
+      </c>
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
@@ -2512,7 +2758,7 @@
       <c r="AG43" s="8"/>
     </row>
     <row r="44" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="18" t="s">
         <v>100</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2541,9 +2787,15 @@
       <c r="M44" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="O44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P44" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="1" t="s">
         <v>107</v>
       </c>
@@ -2570,9 +2822,15 @@
       <c r="M45" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="O45" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P45" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="1" t="s">
         <v>112</v>
       </c>
@@ -2599,9 +2857,15 @@
       <c r="M46" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="O46" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P46" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="1" t="s">
         <v>117</v>
       </c>
@@ -2616,112 +2880,134 @@
         <v>119</v>
       </c>
       <c r="N47" s="1"/>
-      <c r="O47" s="1" t="s">
+      <c r="O47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P47" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="P47" s="2"/>
-    </row>
-    <row r="48" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="O48" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P48" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O49" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P49" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
+      <c r="B50" s="1" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="O50" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P50" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N51" s="1"/>
-      <c r="O51" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P51" s="2"/>
+      <c r="O51" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="P51" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="52" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L52" s="2"/>
       <c r="M52" s="1" t="s">
@@ -2730,56 +3016,72 @@
       <c r="N52" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="O52" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P52" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O53" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P53" s="2"/>
+      <c r="O53" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="P53" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="54" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O54" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P54" s="2"/>
+      <c r="O54" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="P54" s="30" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="55" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K55" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="L55" s="2"/>
       <c r="M55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="O55" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P55" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="9" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="56" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="9" t="s">
-        <v>145</v>
-      </c>
       <c r="C56" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="9"/>
@@ -2787,15 +3089,19 @@
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
       <c r="K56" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L56" s="9"/>
       <c r="M56" s="10"/>
       <c r="N56" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
+        <v>146</v>
+      </c>
+      <c r="O56" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P56" s="30" t="b">
+        <v>0</v>
+      </c>
       <c r="Q56" s="10"/>
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
@@ -2815,30 +3121,34 @@
       <c r="AG56" s="10"/>
     </row>
     <row r="57" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L57" s="9"/>
       <c r="M57" s="10"/>
       <c r="N57" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="O57" s="10"/>
-      <c r="P57" s="10"/>
+        <v>146</v>
+      </c>
+      <c r="O57" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P57" s="30" t="b">
+        <v>0</v>
+      </c>
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
@@ -2858,22 +3168,22 @@
       <c r="AG57" s="10"/>
     </row>
     <row r="58" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="G58" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>24</v>
@@ -2881,15 +3191,19 @@
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
       <c r="K58" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L58" s="9"/>
       <c r="M58" s="10"/>
       <c r="N58" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="O58" s="10"/>
-      <c r="P58" s="10"/>
+        <v>146</v>
+      </c>
+      <c r="O58" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="P58" s="30" t="b">
+        <v>1</v>
+      </c>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
@@ -2909,9 +3223,9 @@
       <c r="AG58" s="10"/>
     </row>
     <row r="59" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>16</v>
@@ -2920,21 +3234,25 @@
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="O59" s="9"/>
-      <c r="P59" s="9"/>
+        <v>146</v>
+      </c>
+      <c r="O59" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="P59" s="30" t="b">
+        <v>0</v>
+      </c>
       <c r="Q59" s="9"/>
       <c r="R59" s="9"/>
       <c r="S59" s="9"/>
@@ -2954,40 +3272,42 @@
       <c r="AG59" s="9"/>
     </row>
     <row r="60" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H60" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="I60" s="10"/>
       <c r="J60" s="10"/>
       <c r="K60" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L60" s="9"/>
       <c r="M60" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="N60" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="O60" s="10"/>
-      <c r="P60" s="10"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P60" s="30" t="b">
+        <v>0</v>
+      </c>
       <c r="Q60" s="10"/>
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
@@ -3007,22 +3327,22 @@
       <c r="AG60" s="10"/>
     </row>
     <row r="61" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="20"/>
       <c r="B61" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G61" s="12" t="s">
         <v>165</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>166</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>24</v>
@@ -3030,15 +3350,17 @@
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
       <c r="K61" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L61" s="12"/>
       <c r="M61" s="11"/>
-      <c r="N61" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="P61" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="Q61" s="11"/>
       <c r="R61" s="11"/>
       <c r="S61" s="11"/>
@@ -3058,41 +3380,41 @@
       <c r="AG61" s="11"/>
     </row>
     <row r="62" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>32</v>
       </c>
       <c r="M62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="N62" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="N62" s="1" t="s">
+    </row>
+    <row r="63" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="19"/>
+      <c r="B63" s="1" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="63" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>32</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N63" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="19"/>
+      <c r="A64" s="20"/>
       <c r="B64" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>16</v>
@@ -3101,13 +3423,13 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
       <c r="K64" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
@@ -3133,130 +3455,130 @@
       <c r="AG64" s="8"/>
     </row>
     <row r="65" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="19"/>
+      <c r="B66" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="L65" s="2"/>
-    </row>
-    <row r="66" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H66" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I66" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="K66" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="19"/>
+      <c r="B67" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="L66" s="2"/>
-    </row>
-    <row r="67" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H67" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="K67" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="19"/>
+      <c r="B68" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="L67" s="2"/>
-    </row>
-    <row r="68" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
-      <c r="B68" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H68" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="K68" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="L68" s="2"/>
-    </row>
-    <row r="69" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
-      <c r="B69" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H69" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I69" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="K69" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="19"/>
+      <c r="B70" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="L69" s="2"/>
-    </row>
-    <row r="70" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
-      <c r="B70" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>32</v>
       </c>
       <c r="M71" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
+      <c r="B72" s="8" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="72" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
-      <c r="B72" s="8" t="s">
-        <v>193</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>32</v>
@@ -3271,10 +3593,10 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N72" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O72" s="8"/>
       <c r="P72" s="8"/>
@@ -3298,33 +3620,39 @@
     </row>
     <row r="73" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
+      </c>
+      <c r="O74" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P74" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>22</v>
@@ -3336,15 +3664,19 @@
       <c r="I75" s="10"/>
       <c r="J75" s="10"/>
       <c r="K75" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L75" s="9"/>
       <c r="M75" s="10"/>
       <c r="N75" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="O75" s="10"/>
-      <c r="P75" s="10"/>
+        <v>201</v>
+      </c>
+      <c r="O75" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P75" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="Q75" s="10"/>
       <c r="R75" s="10"/>
       <c r="S75" s="10"/>
@@ -3366,7 +3698,7 @@
     <row r="76" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>22</v>
@@ -3378,15 +3710,19 @@
       <c r="I76" s="10"/>
       <c r="J76" s="10"/>
       <c r="K76" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L76" s="9"/>
       <c r="M76" s="10"/>
       <c r="N76" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="O76" s="10"/>
-      <c r="P76" s="10"/>
+        <v>204</v>
+      </c>
+      <c r="O76" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P76" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="Q76" s="10"/>
       <c r="R76" s="10"/>
       <c r="S76" s="10"/>
@@ -3407,19 +3743,25 @@
     </row>
     <row r="77" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>32</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
+      </c>
+      <c r="O77" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P77" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="15"/>
       <c r="B78" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>32</v>
@@ -3434,13 +3776,17 @@
       <c r="K78" s="15"/>
       <c r="L78" s="15"/>
       <c r="M78" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="N78" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="N78" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="O78" s="15"/>
-      <c r="P78" s="15"/>
+      <c r="O78" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="P78" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
       <c r="S78" s="15"/>
@@ -3460,11 +3806,11 @@
       <c r="AG78" s="15"/>
     </row>
     <row r="79" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="21" t="s">
+      <c r="A79" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B79" s="13" t="s">
         <v>211</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>212</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -3499,9 +3845,9 @@
       <c r="AG79" s="13"/>
     </row>
     <row r="80" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="18"/>
+      <c r="A80" s="19"/>
       <c r="B80" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
@@ -3536,9 +3882,9 @@
       <c r="AG80" s="13"/>
     </row>
     <row r="81" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="18"/>
+      <c r="A81" s="19"/>
       <c r="B81" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -3573,9 +3919,9 @@
       <c r="AG81" s="13"/>
     </row>
     <row r="82" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
+      <c r="A82" s="19"/>
       <c r="B82" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
@@ -3610,9 +3956,9 @@
       <c r="AG82" s="13"/>
     </row>
     <row r="83" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
+      <c r="A83" s="19"/>
       <c r="B83" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>19</v>
@@ -3653,9 +3999,9 @@
       <c r="AG83" s="13"/>
     </row>
     <row r="84" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
+      <c r="A84" s="19"/>
       <c r="B84" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>22</v>
@@ -3692,7 +4038,7 @@
       <c r="AG84" s="13"/>
     </row>
     <row r="85" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
+      <c r="A85" s="20"/>
       <c r="B85" s="15" t="s">
         <v>100</v>
       </c>
@@ -3703,7 +4049,7 @@
       <c r="E85" s="15"/>
       <c r="F85" s="15"/>
       <c r="G85" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H85" s="15"/>
       <c r="I85" s="15"/>
@@ -3733,41 +4079,41 @@
       <c r="AG85" s="15"/>
     </row>
     <row r="88" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="B88" s="18"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
-      <c r="J88" s="18"/>
-      <c r="K88" s="18"/>
-      <c r="L88" s="18"/>
-      <c r="M88" s="18"/>
-      <c r="N88" s="18"/>
-      <c r="O88" s="18"/>
-      <c r="P88" s="18"/>
-      <c r="Q88" s="18"/>
-      <c r="R88" s="18"/>
-      <c r="S88" s="18"/>
-      <c r="T88" s="18"/>
-      <c r="U88" s="18"/>
-      <c r="V88" s="18"/>
-      <c r="W88" s="18"/>
-      <c r="X88" s="18"/>
-      <c r="Y88" s="18"/>
-      <c r="Z88" s="18"/>
-      <c r="AA88" s="18"/>
-      <c r="AB88" s="18"/>
-      <c r="AC88" s="18"/>
-      <c r="AD88" s="18"/>
-      <c r="AE88" s="18"/>
-      <c r="AF88" s="18"/>
-      <c r="AG88" s="18"/>
+      <c r="A88" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
+      <c r="J88" s="19"/>
+      <c r="K88" s="19"/>
+      <c r="L88" s="19"/>
+      <c r="M88" s="19"/>
+      <c r="N88" s="19"/>
+      <c r="O88" s="19"/>
+      <c r="P88" s="19"/>
+      <c r="Q88" s="19"/>
+      <c r="R88" s="19"/>
+      <c r="S88" s="19"/>
+      <c r="T88" s="19"/>
+      <c r="U88" s="19"/>
+      <c r="V88" s="19"/>
+      <c r="W88" s="19"/>
+      <c r="X88" s="19"/>
+      <c r="Y88" s="19"/>
+      <c r="Z88" s="19"/>
+      <c r="AA88" s="19"/>
+      <c r="AB88" s="19"/>
+      <c r="AC88" s="19"/>
+      <c r="AD88" s="19"/>
+      <c r="AE88" s="19"/>
+      <c r="AF88" s="19"/>
+      <c r="AG88" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
update camera setting controller
</commit_message>
<xml_diff>
--- a/design/Widgets list.xlsx
+++ b/design/Widgets list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroscopyInnovation\Documents\GitHub\ASLM\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\python\tkinter\workspace\ASLM\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2FAE3-A467-48EC-8D08-254B4F69EEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F32507E-B9EF-4552-B3EE-DD2140C5A79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="2030" windowWidth="38400" windowHeight="18190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="262">
   <si>
     <t>view</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>Center_Y</t>
-  </si>
-  <si>
-    <t>Use_Pixels</t>
   </si>
   <si>
     <t>Button</t>
@@ -720,9 +717,6 @@
     <t>Normal' or 'Light-Sheet'</t>
   </si>
   <si>
-    <t>If == 'Normal', Readout Direction and Number of Pixels Disabled.</t>
-  </si>
-  <si>
     <t>Top-to-Bottom' or 'Bottom-to-Top'</t>
   </si>
   <si>
@@ -741,9 +735,6 @@
     <t>readout_time</t>
   </si>
   <si>
-    <t>images_to_average</t>
-  </si>
-  <si>
     <t>Retrieve current exposure time for the active channel in milliseconds</t>
   </si>
   <si>
@@ -838,13 +829,42 @@
   </si>
   <si>
     <t>model.camera_calculate_readout_time()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If == 'Normal', Readout Direction and Number of Pixels Disabled.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recalculate Readout time</t>
+    </r>
+  </si>
+  <si>
+    <t>Recalculate readout time</t>
+  </si>
+  <si>
+    <t>Recalculate Readout time
+Tell central controller to update channels setting</t>
+  </si>
+  <si>
+    <t>frames_to_average</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -936,6 +956,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -990,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,6 +1070,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1064,26 +1112,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1305,10 +1341,10 @@
   </sheetPr>
   <dimension ref="A1:AG88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3750" ySplit="14320" topLeftCell="G1" activePane="topRight"/>
-      <selection activeCell="A3" sqref="A3:A20"/>
-      <selection pane="topRight" activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <pane xSplit="3750" ySplit="14320" topLeftCell="N1"/>
+      <selection activeCell="B8" sqref="B8"/>
+      <selection pane="topRight" activeCell="O6" sqref="O6"/>
       <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
@@ -1335,116 +1371,116 @@
     <col min="18" max="16384" width="12.6328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="26" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
+    <row r="1" spans="1:33" s="19" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="23" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="M1" s="23" t="s">
+      <c r="L1" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-    </row>
-    <row r="2" spans="1:33" s="26" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+    </row>
+    <row r="2" spans="1:33" s="19" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-    </row>
-    <row r="3" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+    </row>
+    <row r="3" spans="1:33" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1455,74 +1491,75 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>251</v>
-      </c>
       <c r="H3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="I3" s="27" t="s">
-        <v>179</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="N3" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="O3" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" s="27" t="b">
+      <c r="M3" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="O3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="20" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="H4" s="27" t="s">
+      <c r="E4" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="I4" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="27" t="s">
-        <v>179</v>
-      </c>
       <c r="K4" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="N4" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="O4" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" s="27" t="b">
+      <c r="M4" s="33"/>
+      <c r="N4" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="O4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="20" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1532,141 +1569,147 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>250</v>
+      <c r="E5" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>247</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="L5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="O5" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="25" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="L5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="28" t="s">
-        <v>252</v>
+      <c r="E6" s="21" t="s">
+        <v>249</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="28" t="s">
-        <v>254</v>
+      <c r="G6" s="21" t="s">
+        <v>251</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="L6" s="27" t="b">
-        <v>1</v>
+        <v>225</v>
+      </c>
+      <c r="L6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>259</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P6" s="28" t="b">
+      <c r="P6" s="21" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="28" t="s">
-        <v>251</v>
+      <c r="E7" s="21" t="s">
+        <v>248</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="28" t="s">
-        <v>251</v>
+      <c r="G7" s="21" t="s">
+        <v>248</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="O7" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="P7" s="28" t="s">
-        <v>251</v>
+        <v>226</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="28" t="s">
-        <v>258</v>
+      <c r="A8" s="26"/>
+      <c r="B8" s="21" t="s">
+        <v>255</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="28" t="s">
-        <v>251</v>
+      <c r="E8" s="21" t="s">
+        <v>248</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="28" t="s">
-        <v>251</v>
+      <c r="G8" s="21" t="s">
+        <v>248</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="L8" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="N8" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="O8" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="P8" s="28" t="s">
-        <v>251</v>
+        <v>227</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="1" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
@@ -1674,8 +1717,8 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="28" t="s">
-        <v>253</v>
+      <c r="E9" s="21" t="s">
+        <v>250</v>
       </c>
       <c r="F9" s="1">
         <v>8</v>
@@ -1692,17 +1735,17 @@
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="O9" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" s="27" t="b">
+        <v>235</v>
+      </c>
+      <c r="O9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="20" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:33" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1716,7 +1759,7 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1727,34 +1770,34 @@
         <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G11" s="1">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O11" s="1" t="b">
         <v>0</v>
@@ -1764,45 +1807,45 @@
       </c>
     </row>
     <row r="12" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D12" s="1">
         <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G12" s="1">
         <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O12" s="1" t="b">
         <v>0</v>
@@ -1812,7 +1855,7 @@
       </c>
     </row>
     <row r="13" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1820,39 +1863,39 @@
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="O13" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="P13" s="27" t="s">
-        <v>251</v>
+        <v>241</v>
+      </c>
+      <c r="O13" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1860,39 +1903,39 @@
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="O14" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="P14" s="27" t="s">
-        <v>251</v>
+        <v>241</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="P14" s="20" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1909,29 +1952,29 @@
         <v>1024</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="O15" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="P15" s="27" t="s">
-        <v>251</v>
+        <v>238</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="P15" s="20" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1948,62 +1991,62 @@
         <v>1024</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="O16" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="P16" s="27" t="s">
-        <v>251</v>
+        <v>238</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="P16" s="20" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="K17" s="28" t="s">
-        <v>251</v>
+        <v>231</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>248</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O17" s="3" t="b">
         <v>0</v>
@@ -2013,40 +2056,40 @@
       </c>
     </row>
     <row r="18" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="1">
         <v>1600</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="K18" s="28" t="s">
-        <v>251</v>
+        <v>231</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>248</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O18" s="3" t="b">
         <v>0</v>
@@ -2056,40 +2099,40 @@
       </c>
     </row>
     <row r="19" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="1">
         <v>1024</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="K19" s="28" t="s">
-        <v>251</v>
+        <v>231</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>248</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O19" s="3" t="b">
         <v>0</v>
@@ -2099,41 +2142,41 @@
       </c>
     </row>
     <row r="20" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="8">
         <v>512</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="J20" s="8"/>
-      <c r="K20" s="29" t="s">
-        <v>251</v>
+      <c r="K20" s="22" t="s">
+        <v>248</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O20" s="8" t="b">
         <v>0</v>
@@ -2160,65 +2203,65 @@
       <c r="AG20" s="8"/>
     </row>
     <row r="21" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="L21" s="2"/>
       <c r="N21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="O21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P21" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L22" s="2"/>
       <c r="N22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O22" s="17" t="b">
         <v>1</v>
@@ -2228,30 +2271,30 @@
       </c>
     </row>
     <row r="23" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L23" s="2"/>
       <c r="N23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O23" s="17" t="b">
         <v>1</v>
@@ -2261,30 +2304,30 @@
       </c>
     </row>
     <row r="24" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L24" s="2"/>
       <c r="N24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O24" s="17" t="b">
         <v>1</v>
@@ -2294,30 +2337,30 @@
       </c>
     </row>
     <row r="25" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L25" s="2"/>
       <c r="N25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O25" s="17" t="b">
         <v>1</v>
@@ -2327,28 +2370,28 @@
       </c>
     </row>
     <row r="26" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="1"/>
@@ -2360,28 +2403,28 @@
       </c>
     </row>
     <row r="27" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="1"/>
@@ -2393,28 +2436,28 @@
       </c>
     </row>
     <row r="28" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="1"/>
@@ -2426,28 +2469,28 @@
       </c>
     </row>
     <row r="29" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="1"/>
@@ -2459,117 +2502,117 @@
       </c>
     </row>
     <row r="30" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="2"/>
       <c r="M30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O30" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P30" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="2"/>
       <c r="M31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O31" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O31" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P31" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="2"/>
       <c r="M32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O32" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O32" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P32" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="2"/>
       <c r="M33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O33" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O33" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P33" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="2"/>
       <c r="M34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O34" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O34" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P34" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="2"/>
       <c r="M35" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O35" s="17" t="b">
         <v>1</v>
@@ -2579,17 +2622,17 @@
       </c>
     </row>
     <row r="36" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="2"/>
       <c r="M36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O36" s="17" t="b">
         <v>1</v>
@@ -2599,17 +2642,17 @@
       </c>
     </row>
     <row r="37" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="2"/>
       <c r="M37" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O37" s="17" t="b">
         <v>1</v>
@@ -2619,17 +2662,17 @@
       </c>
     </row>
     <row r="38" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="2"/>
       <c r="M38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O38" s="17" t="b">
         <v>1</v>
@@ -2639,17 +2682,17 @@
       </c>
     </row>
     <row r="39" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="2"/>
       <c r="M39" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O39" s="17" t="b">
         <v>1</v>
@@ -2659,66 +2702,66 @@
       </c>
     </row>
     <row r="40" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M40" s="1" t="s">
+      <c r="O40" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P40" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
+      <c r="B41" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O40" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P40" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M41" s="1" t="s">
+      <c r="O41" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O41" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P41" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M42" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M42" s="1" t="s">
+      <c r="O42" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
+      <c r="B43" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="O42" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="P42" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="C43" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -2730,7 +2773,7 @@
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N43" s="8"/>
       <c r="O43" s="17" t="b">
@@ -2758,69 +2801,69 @@
       <c r="AG43" s="8"/>
     </row>
     <row r="44" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P44" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="26"/>
+      <c r="B45" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="O44" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P44" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="H45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O45" s="3" t="b">
         <v>0</v>
@@ -2830,32 +2873,32 @@
       </c>
     </row>
     <row r="46" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O46" s="3" t="b">
         <v>0</v>
@@ -2865,19 +2908,19 @@
       </c>
     </row>
     <row r="47" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L47" s="2"/>
       <c r="M47" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1" t="b">
@@ -2888,22 +2931,22 @@
       </c>
     </row>
     <row r="48" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O48" s="3" t="b">
         <v>0</v>
@@ -2913,54 +2956,54 @@
       </c>
     </row>
     <row r="49" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O49" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P49" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="26"/>
+      <c r="B50" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="O49" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P49" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="B50" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O50" s="3" t="b">
         <v>0</v>
@@ -2970,44 +3013,44 @@
       </c>
     </row>
     <row r="51" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N51" s="1"/>
-      <c r="O51" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="P51" s="28" t="s">
-        <v>251</v>
+      <c r="O51" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="P51" s="21" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L52" s="2"/>
       <c r="M52" s="1" t="s">
@@ -3024,64 +3067,64 @@
       </c>
     </row>
     <row r="53" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O53" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="P53" s="28" t="s">
-        <v>251</v>
+      <c r="O53" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="P53" s="21" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O54" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="P54" s="30" t="s">
-        <v>251</v>
+      <c r="O54" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="P54" s="23" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="55" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K55" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="L55" s="2"/>
       <c r="M55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O55" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P55" s="23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="26"/>
+      <c r="B56" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="O55" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="P55" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="9" t="s">
-        <v>144</v>
-      </c>
       <c r="C56" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="9"/>
@@ -3089,17 +3132,17 @@
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
       <c r="K56" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L56" s="9"/>
       <c r="M56" s="10"/>
       <c r="N56" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="O56" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="P56" s="30" t="b">
+        <v>145</v>
+      </c>
+      <c r="O56" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P56" s="23" t="b">
         <v>0</v>
       </c>
       <c r="Q56" s="10"/>
@@ -3121,32 +3164,32 @@
       <c r="AG56" s="10"/>
     </row>
     <row r="57" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L57" s="9"/>
       <c r="M57" s="10"/>
       <c r="N57" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="O57" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="P57" s="30" t="b">
+        <v>145</v>
+      </c>
+      <c r="O57" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P57" s="23" t="b">
         <v>0</v>
       </c>
       <c r="Q57" s="10"/>
@@ -3168,22 +3211,22 @@
       <c r="AG57" s="10"/>
     </row>
     <row r="58" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G58" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>24</v>
@@ -3191,17 +3234,17 @@
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
       <c r="K58" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L58" s="9"/>
       <c r="M58" s="10"/>
       <c r="N58" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="O58" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="P58" s="30" t="b">
+        <v>145</v>
+      </c>
+      <c r="O58" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P58" s="23" t="b">
         <v>1</v>
       </c>
       <c r="Q58" s="10"/>
@@ -3223,9 +3266,9 @@
       <c r="AG58" s="10"/>
     </row>
     <row r="59" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>16</v>
@@ -3234,23 +3277,23 @@
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="O59" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="P59" s="30" t="b">
+        <v>145</v>
+      </c>
+      <c r="O59" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P59" s="23" t="b">
         <v>0</v>
       </c>
       <c r="Q59" s="9"/>
@@ -3272,40 +3315,40 @@
       <c r="AG59" s="9"/>
     </row>
     <row r="60" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H60" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="I60" s="10"/>
       <c r="J60" s="10"/>
       <c r="K60" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L60" s="9"/>
       <c r="M60" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N60" s="9"/>
-      <c r="O60" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="P60" s="30" t="b">
+      <c r="O60" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P60" s="23" t="b">
         <v>0</v>
       </c>
       <c r="Q60" s="10"/>
@@ -3327,22 +3370,22 @@
       <c r="AG60" s="10"/>
     </row>
     <row r="61" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G61" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>24</v>
@@ -3350,15 +3393,15 @@
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
       <c r="K61" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L61" s="12"/>
       <c r="M61" s="11"/>
       <c r="N61" s="12"/>
-      <c r="O61" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="P61" s="31" t="b">
+      <c r="O61" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P61" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Q61" s="11"/>
@@ -3380,41 +3423,41 @@
       <c r="AG61" s="11"/>
     </row>
     <row r="62" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M62" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M62" s="1" t="s">
+      <c r="N62" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="N62" s="1" t="s">
+    </row>
+    <row r="63" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="26"/>
+      <c r="B63" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="63" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M63" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="N63" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
+      <c r="A64" s="27"/>
       <c r="B64" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>16</v>
@@ -3423,13 +3466,13 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
       <c r="K64" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
@@ -3455,133 +3498,133 @@
       <c r="AG64" s="8"/>
     </row>
     <row r="65" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="26"/>
+      <c r="B66" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="L65" s="2"/>
-    </row>
-    <row r="66" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="19"/>
-      <c r="B66" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H66" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I66" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="K66" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="26"/>
+      <c r="B67" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="L66" s="2"/>
-    </row>
-    <row r="67" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
-      <c r="B67" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H67" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="K67" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="26"/>
+      <c r="B68" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="L67" s="2"/>
-    </row>
-    <row r="68" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H68" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="K68" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="26"/>
+      <c r="B69" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="L68" s="2"/>
-    </row>
-    <row r="69" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H69" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I69" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="K69" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="26"/>
+      <c r="B70" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="L69" s="2"/>
-    </row>
-    <row r="70" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
-      <c r="B70" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M71" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M71" s="1" t="s">
+    </row>
+    <row r="72" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="27"/>
+      <c r="B72" s="8" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="72" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="8" t="s">
-        <v>192</v>
-      </c>
       <c r="C72" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
@@ -3593,10 +3636,10 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N72" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O72" s="8"/>
       <c r="P72" s="8"/>
@@ -3620,27 +3663,27 @@
     </row>
     <row r="73" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O74" s="3" t="b">
         <v>1</v>
@@ -3652,7 +3695,7 @@
     <row r="75" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>22</v>
@@ -3664,12 +3707,12 @@
       <c r="I75" s="10"/>
       <c r="J75" s="10"/>
       <c r="K75" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L75" s="9"/>
       <c r="M75" s="10"/>
       <c r="N75" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O75" s="10" t="b">
         <v>1</v>
@@ -3698,7 +3741,7 @@
     <row r="76" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>22</v>
@@ -3710,12 +3753,12 @@
       <c r="I76" s="10"/>
       <c r="J76" s="10"/>
       <c r="K76" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L76" s="9"/>
       <c r="M76" s="10"/>
       <c r="N76" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O76" s="10" t="b">
         <v>1</v>
@@ -3743,13 +3786,13 @@
     </row>
     <row r="77" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M77" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M77" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="O77" s="3" t="b">
         <v>1</v>
@@ -3761,10 +3804,10 @@
     <row r="78" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="15"/>
       <c r="B78" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D78" s="15"/>
       <c r="E78" s="15"/>
@@ -3776,10 +3819,10 @@
       <c r="K78" s="15"/>
       <c r="L78" s="15"/>
       <c r="M78" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="N78" s="16" t="s">
         <v>208</v>
-      </c>
-      <c r="N78" s="16" t="s">
-        <v>209</v>
       </c>
       <c r="O78" s="15" t="b">
         <v>0</v>
@@ -3806,11 +3849,11 @@
       <c r="AG78" s="15"/>
     </row>
     <row r="79" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" s="13" t="s">
         <v>210</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>211</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -3845,9 +3888,9 @@
       <c r="AG79" s="13"/>
     </row>
     <row r="80" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
@@ -3882,9 +3925,9 @@
       <c r="AG80" s="13"/>
     </row>
     <row r="81" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="19"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -3919,9 +3962,9 @@
       <c r="AG81" s="13"/>
     </row>
     <row r="82" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="19"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
@@ -3956,9 +3999,9 @@
       <c r="AG82" s="13"/>
     </row>
     <row r="83" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="19"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>19</v>
@@ -3999,9 +4042,9 @@
       <c r="AG83" s="13"/>
     </row>
     <row r="84" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>22</v>
@@ -4038,9 +4081,9 @@
       <c r="AG84" s="13"/>
     </row>
     <row r="85" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>22</v>
@@ -4049,7 +4092,7 @@
       <c r="E85" s="15"/>
       <c r="F85" s="15"/>
       <c r="G85" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H85" s="15"/>
       <c r="I85" s="15"/>
@@ -4079,41 +4122,41 @@
       <c r="AG85" s="15"/>
     </row>
     <row r="88" spans="1:33" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="19"/>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
-      <c r="J88" s="19"/>
-      <c r="K88" s="19"/>
-      <c r="L88" s="19"/>
-      <c r="M88" s="19"/>
-      <c r="N88" s="19"/>
-      <c r="O88" s="19"/>
-      <c r="P88" s="19"/>
-      <c r="Q88" s="19"/>
-      <c r="R88" s="19"/>
-      <c r="S88" s="19"/>
-      <c r="T88" s="19"/>
-      <c r="U88" s="19"/>
-      <c r="V88" s="19"/>
-      <c r="W88" s="19"/>
-      <c r="X88" s="19"/>
-      <c r="Y88" s="19"/>
-      <c r="Z88" s="19"/>
-      <c r="AA88" s="19"/>
-      <c r="AB88" s="19"/>
-      <c r="AC88" s="19"/>
-      <c r="AD88" s="19"/>
-      <c r="AE88" s="19"/>
-      <c r="AF88" s="19"/>
-      <c r="AG88" s="19"/>
+      <c r="A88" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="26"/>
+      <c r="I88" s="26"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="26"/>
+      <c r="L88" s="26"/>
+      <c r="M88" s="26"/>
+      <c r="N88" s="26"/>
+      <c r="O88" s="26"/>
+      <c r="P88" s="26"/>
+      <c r="Q88" s="26"/>
+      <c r="R88" s="26"/>
+      <c r="S88" s="26"/>
+      <c r="T88" s="26"/>
+      <c r="U88" s="26"/>
+      <c r="V88" s="26"/>
+      <c r="W88" s="26"/>
+      <c r="X88" s="26"/>
+      <c r="Y88" s="26"/>
+      <c r="Z88" s="26"/>
+      <c r="AA88" s="26"/>
+      <c r="AB88" s="26"/>
+      <c r="AC88" s="26"/>
+      <c r="AD88" s="26"/>
+      <c r="AE88" s="26"/>
+      <c r="AF88" s="26"/>
+      <c r="AG88" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>